<commit_message>
dual working on HF; dual has a bug on ND
</commit_message>
<xml_diff>
--- a/data/SiouxFalls/SF_creation.xlsx
+++ b/data/SiouxFalls/SF_creation.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaellevin/Documents/NetBeansProjects/CNDP/data/SiouxFalls/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michael/Documents/NetbeansProjects/DNDP/data/SiouxFalls/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44434944-44A5-6D41-8BDE-2C3DB2DB0BEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{280016A7-C77D-9743-88FC-9B9E616969C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1160" yWindow="1440" windowWidth="27640" windowHeight="16440" xr2:uid="{418FED77-12DA-7B43-B3FF-D0E20B702B8C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -519,7 +519,7 @@
   <dimension ref="A1:P85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:M1048576"/>
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -660,7 +660,7 @@
         <v>1</v>
       </c>
       <c r="L10">
-        <f ca="1">IF(COUNTIF(O$10:O$29, P10)&gt;0, RAND()*0.5, 0)</f>
+        <f ca="1">IF(COUNTIF(O$10:O$19, P10)&gt;0, RAND()*0.5, 0)</f>
         <v>0</v>
       </c>
       <c r="M10" t="s">
@@ -671,7 +671,7 @@
       </c>
       <c r="P10" cm="1">
         <f t="array" aca="1" ref="P10:P85" ca="1">_xlfn.SORTBY(_xlfn.SEQUENCE(76),_xlfn.RANDARRAY(76))</f>
-        <v>59</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
@@ -706,8 +706,8 @@
         <v>1</v>
       </c>
       <c r="L11">
-        <f t="shared" ref="L11:L74" ca="1" si="0">IF(COUNTIF(O$10:O$29, P11)&gt;0, RAND()*0.5, 0)</f>
-        <v>0.21144677205401513</v>
+        <f t="shared" ref="L11:L74" ca="1" si="0">IF(COUNTIF(O$10:O$19, P11)&gt;0, RAND()*0.5, 0)</f>
+        <v>0</v>
       </c>
       <c r="M11" t="s">
         <v>5</v>
@@ -718,7 +718,7 @@
       </c>
       <c r="P11">
         <f ca="1"/>
-        <v>2</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
@@ -801,7 +801,7 @@
       </c>
       <c r="L13">
         <f t="shared" ca="1" si="0"/>
-        <v>0.37445636393969939</v>
+        <v>0.40508213798720383</v>
       </c>
       <c r="M13" t="s">
         <v>5</v>
@@ -812,7 +812,7 @@
       </c>
       <c r="P13">
         <f ca="1"/>
-        <v>18</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
@@ -859,7 +859,7 @@
       </c>
       <c r="P14">
         <f ca="1"/>
-        <v>27</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
@@ -906,7 +906,7 @@
       </c>
       <c r="P15">
         <f ca="1"/>
-        <v>33</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
@@ -953,7 +953,7 @@
       </c>
       <c r="P16">
         <f ca="1"/>
-        <v>51</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="2:16" x14ac:dyDescent="0.2">
@@ -1000,7 +1000,7 @@
       </c>
       <c r="P17">
         <f ca="1"/>
-        <v>39</v>
+        <v>64</v>
       </c>
     </row>
     <row r="18" spans="2:16" x14ac:dyDescent="0.2">
@@ -1047,7 +1047,7 @@
       </c>
       <c r="P18">
         <f ca="1"/>
-        <v>36</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="2:16" x14ac:dyDescent="0.2">
@@ -1094,7 +1094,7 @@
       </c>
       <c r="P19">
         <f ca="1"/>
-        <v>52</v>
+        <v>13</v>
       </c>
     </row>
     <row r="20" spans="2:16" x14ac:dyDescent="0.2">
@@ -1141,7 +1141,7 @@
       </c>
       <c r="P20">
         <f ca="1"/>
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="21" spans="2:16" x14ac:dyDescent="0.2">
@@ -1188,7 +1188,7 @@
       </c>
       <c r="P21">
         <f ca="1"/>
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="22" spans="2:16" x14ac:dyDescent="0.2">
@@ -1235,7 +1235,7 @@
       </c>
       <c r="P22">
         <f ca="1"/>
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="23" spans="2:16" x14ac:dyDescent="0.2">
@@ -1282,7 +1282,7 @@
       </c>
       <c r="P23">
         <f ca="1"/>
-        <v>44</v>
+        <v>17</v>
       </c>
     </row>
     <row r="24" spans="2:16" x14ac:dyDescent="0.2">
@@ -1329,7 +1329,7 @@
       </c>
       <c r="P24">
         <f ca="1"/>
-        <v>75</v>
+        <v>12</v>
       </c>
     </row>
     <row r="25" spans="2:16" x14ac:dyDescent="0.2">
@@ -1365,7 +1365,7 @@
       </c>
       <c r="L25">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>0.37144890327851909</v>
       </c>
       <c r="M25" t="s">
         <v>5</v>
@@ -1376,7 +1376,7 @@
       </c>
       <c r="P25">
         <f ca="1"/>
-        <v>72</v>
+        <v>5</v>
       </c>
     </row>
     <row r="26" spans="2:16" x14ac:dyDescent="0.2">
@@ -1412,7 +1412,7 @@
       </c>
       <c r="L26">
         <f t="shared" ca="1" si="0"/>
-        <v>0.31804211181788306</v>
+        <v>0</v>
       </c>
       <c r="M26" t="s">
         <v>5</v>
@@ -1423,7 +1423,7 @@
       </c>
       <c r="P26">
         <f ca="1"/>
-        <v>15</v>
+        <v>70</v>
       </c>
     </row>
     <row r="27" spans="2:16" x14ac:dyDescent="0.2">
@@ -1459,7 +1459,7 @@
       </c>
       <c r="L27">
         <f t="shared" ca="1" si="0"/>
-        <v>0.33007732604903733</v>
+        <v>0</v>
       </c>
       <c r="M27" t="s">
         <v>5</v>
@@ -1470,7 +1470,7 @@
       </c>
       <c r="P27">
         <f ca="1"/>
-        <v>4</v>
+        <v>72</v>
       </c>
     </row>
     <row r="28" spans="2:16" x14ac:dyDescent="0.2">
@@ -1506,7 +1506,7 @@
       </c>
       <c r="L28">
         <f t="shared" ca="1" si="0"/>
-        <v>0.13239282429354593</v>
+        <v>0</v>
       </c>
       <c r="M28" t="s">
         <v>5</v>
@@ -1517,7 +1517,7 @@
       </c>
       <c r="P28">
         <f ca="1"/>
-        <v>3</v>
+        <v>52</v>
       </c>
     </row>
     <row r="29" spans="2:16" x14ac:dyDescent="0.2">
@@ -1564,7 +1564,7 @@
       </c>
       <c r="P29">
         <f ca="1"/>
-        <v>76</v>
+        <v>27</v>
       </c>
     </row>
     <row r="30" spans="2:16" x14ac:dyDescent="0.2">
@@ -1611,7 +1611,7 @@
       </c>
       <c r="P30">
         <f ca="1"/>
-        <v>32</v>
+        <v>11</v>
       </c>
     </row>
     <row r="31" spans="2:16" x14ac:dyDescent="0.2">
@@ -1658,7 +1658,7 @@
       </c>
       <c r="P31">
         <f ca="1"/>
-        <v>35</v>
+        <v>15</v>
       </c>
     </row>
     <row r="32" spans="2:16" x14ac:dyDescent="0.2">
@@ -1694,7 +1694,7 @@
       </c>
       <c r="L32">
         <f t="shared" ca="1" si="0"/>
-        <v>0.19760948217760577</v>
+        <v>0</v>
       </c>
       <c r="M32" t="s">
         <v>5</v>
@@ -1705,7 +1705,7 @@
       </c>
       <c r="P32">
         <f ca="1"/>
-        <v>9</v>
+        <v>31</v>
       </c>
     </row>
     <row r="33" spans="2:16" x14ac:dyDescent="0.2">
@@ -1741,7 +1741,7 @@
       </c>
       <c r="L33">
         <f t="shared" ca="1" si="0"/>
-        <v>9.4175040339363747E-3</v>
+        <v>0</v>
       </c>
       <c r="M33" t="s">
         <v>5</v>
@@ -1752,7 +1752,7 @@
       </c>
       <c r="P33">
         <f ca="1"/>
-        <v>16</v>
+        <v>60</v>
       </c>
     </row>
     <row r="34" spans="2:16" x14ac:dyDescent="0.2">
@@ -1799,7 +1799,7 @@
       </c>
       <c r="P34">
         <f ca="1"/>
-        <v>70</v>
+        <v>33</v>
       </c>
     </row>
     <row r="35" spans="2:16" x14ac:dyDescent="0.2">
@@ -1835,7 +1835,7 @@
       </c>
       <c r="L35">
         <f t="shared" ca="1" si="0"/>
-        <v>2.9756050270295764E-2</v>
+        <v>0</v>
       </c>
       <c r="M35" t="s">
         <v>5</v>
@@ -1846,7 +1846,7 @@
       </c>
       <c r="P35">
         <f ca="1"/>
-        <v>7</v>
+        <v>71</v>
       </c>
     </row>
     <row r="36" spans="2:16" x14ac:dyDescent="0.2">
@@ -1893,7 +1893,7 @@
       </c>
       <c r="P36">
         <f ca="1"/>
-        <v>63</v>
+        <v>38</v>
       </c>
     </row>
     <row r="37" spans="2:16" x14ac:dyDescent="0.2">
@@ -1929,7 +1929,7 @@
       </c>
       <c r="L37">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>0.25201978057629731</v>
       </c>
       <c r="M37" t="s">
         <v>5</v>
@@ -1940,7 +1940,7 @@
       </c>
       <c r="P37">
         <f ca="1"/>
-        <v>46</v>
+        <v>8</v>
       </c>
     </row>
     <row r="38" spans="2:16" x14ac:dyDescent="0.2">
@@ -2034,7 +2034,7 @@
       </c>
       <c r="P39">
         <f ca="1"/>
-        <v>38</v>
+        <v>47</v>
       </c>
     </row>
     <row r="40" spans="2:16" x14ac:dyDescent="0.2">
@@ -2070,7 +2070,7 @@
       </c>
       <c r="L40">
         <f t="shared" ca="1" si="0"/>
-        <v>0.38555363256536196</v>
+        <v>0</v>
       </c>
       <c r="M40" t="s">
         <v>5</v>
@@ -2081,7 +2081,7 @@
       </c>
       <c r="P40">
         <f ca="1"/>
-        <v>17</v>
+        <v>44</v>
       </c>
     </row>
     <row r="41" spans="2:16" x14ac:dyDescent="0.2">
@@ -2117,7 +2117,7 @@
       </c>
       <c r="L41">
         <f t="shared" ca="1" si="0"/>
-        <v>0.31961367296097526</v>
+        <v>0</v>
       </c>
       <c r="M41" t="s">
         <v>5</v>
@@ -2128,7 +2128,7 @@
       </c>
       <c r="P41">
         <f ca="1"/>
-        <v>1</v>
+        <v>21</v>
       </c>
     </row>
     <row r="42" spans="2:16" x14ac:dyDescent="0.2">
@@ -2175,7 +2175,7 @@
       </c>
       <c r="P42">
         <f ca="1"/>
-        <v>42</v>
+        <v>34</v>
       </c>
     </row>
     <row r="43" spans="2:16" x14ac:dyDescent="0.2">
@@ -2222,7 +2222,7 @@
       </c>
       <c r="P43">
         <f ca="1"/>
-        <v>43</v>
+        <v>24</v>
       </c>
     </row>
     <row r="44" spans="2:16" x14ac:dyDescent="0.2">
@@ -2258,7 +2258,7 @@
       </c>
       <c r="L44">
         <f t="shared" ca="1" si="0"/>
-        <v>0.31864153097225678</v>
+        <v>0</v>
       </c>
       <c r="M44" t="s">
         <v>5</v>
@@ -2269,7 +2269,7 @@
       </c>
       <c r="P44">
         <f ca="1"/>
-        <v>11</v>
+        <v>22</v>
       </c>
     </row>
     <row r="45" spans="2:16" x14ac:dyDescent="0.2">
@@ -2305,7 +2305,7 @@
       </c>
       <c r="L45">
         <f t="shared" ca="1" si="0"/>
-        <v>6.8758710196253348E-3</v>
+        <v>0</v>
       </c>
       <c r="M45" t="s">
         <v>5</v>
@@ -2316,7 +2316,7 @@
       </c>
       <c r="P45">
         <f ca="1"/>
-        <v>13</v>
+        <v>57</v>
       </c>
     </row>
     <row r="46" spans="2:16" x14ac:dyDescent="0.2">
@@ -2363,7 +2363,7 @@
       </c>
       <c r="P46">
         <f ca="1"/>
-        <v>31</v>
+        <v>54</v>
       </c>
     </row>
     <row r="47" spans="2:16" x14ac:dyDescent="0.2">
@@ -2399,7 +2399,7 @@
       </c>
       <c r="L47">
         <f t="shared" ca="1" si="0"/>
-        <v>0.16935267393041925</v>
+        <v>0</v>
       </c>
       <c r="M47" t="s">
         <v>5</v>
@@ -2410,7 +2410,7 @@
       </c>
       <c r="P47">
         <f ca="1"/>
-        <v>20</v>
+        <v>36</v>
       </c>
     </row>
     <row r="48" spans="2:16" x14ac:dyDescent="0.2">
@@ -2457,7 +2457,7 @@
       </c>
       <c r="P48">
         <f ca="1"/>
-        <v>58</v>
+        <v>26</v>
       </c>
     </row>
     <row r="49" spans="2:16" x14ac:dyDescent="0.2">
@@ -2504,7 +2504,7 @@
       </c>
       <c r="P49">
         <f ca="1"/>
-        <v>61</v>
+        <v>16</v>
       </c>
     </row>
     <row r="50" spans="2:16" x14ac:dyDescent="0.2">
@@ -2551,7 +2551,7 @@
       </c>
       <c r="P50">
         <f ca="1"/>
-        <v>50</v>
+        <v>62</v>
       </c>
     </row>
     <row r="51" spans="2:16" x14ac:dyDescent="0.2">
@@ -2587,7 +2587,7 @@
       </c>
       <c r="L51">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>0.31771492860280659</v>
       </c>
       <c r="M51" t="s">
         <v>5</v>
@@ -2598,7 +2598,7 @@
       </c>
       <c r="P51">
         <f ca="1"/>
-        <v>30</v>
+        <v>2</v>
       </c>
     </row>
     <row r="52" spans="2:16" x14ac:dyDescent="0.2">
@@ -2645,7 +2645,7 @@
       </c>
       <c r="P52">
         <f ca="1"/>
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="53" spans="2:16" x14ac:dyDescent="0.2">
@@ -2681,7 +2681,7 @@
       </c>
       <c r="L53">
         <f t="shared" ca="1" si="0"/>
-        <v>0.42389709415950855</v>
+        <v>0</v>
       </c>
       <c r="M53" t="s">
         <v>5</v>
@@ -2692,7 +2692,7 @@
       </c>
       <c r="P53">
         <f ca="1"/>
-        <v>5</v>
+        <v>32</v>
       </c>
     </row>
     <row r="54" spans="2:16" x14ac:dyDescent="0.2">
@@ -2728,7 +2728,7 @@
       </c>
       <c r="L54">
         <f t="shared" ca="1" si="0"/>
-        <v>0.2144354946299985</v>
+        <v>0</v>
       </c>
       <c r="M54" t="s">
         <v>5</v>
@@ -2739,7 +2739,7 @@
       </c>
       <c r="P54">
         <f ca="1"/>
-        <v>6</v>
+        <v>40</v>
       </c>
     </row>
     <row r="55" spans="2:16" x14ac:dyDescent="0.2">
@@ -2775,7 +2775,7 @@
       </c>
       <c r="L55">
         <f t="shared" ca="1" si="0"/>
-        <v>0.3201972840772942</v>
+        <v>0.40794650256977633</v>
       </c>
       <c r="M55" t="s">
         <v>5</v>
@@ -2786,7 +2786,7 @@
       </c>
       <c r="P55">
         <f ca="1"/>
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="56" spans="2:16" x14ac:dyDescent="0.2">
@@ -2822,7 +2822,7 @@
       </c>
       <c r="L56">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>9.7844361365735821E-2</v>
       </c>
       <c r="M56" t="s">
         <v>5</v>
@@ -2833,7 +2833,7 @@
       </c>
       <c r="P56">
         <f ca="1"/>
-        <v>57</v>
+        <v>3</v>
       </c>
     </row>
     <row r="57" spans="2:16" x14ac:dyDescent="0.2">
@@ -2880,7 +2880,7 @@
       </c>
       <c r="P57">
         <f ca="1"/>
-        <v>68</v>
+        <v>49</v>
       </c>
     </row>
     <row r="58" spans="2:16" x14ac:dyDescent="0.2">
@@ -2927,7 +2927,7 @@
       </c>
       <c r="P58">
         <f ca="1"/>
-        <v>34</v>
+        <v>59</v>
       </c>
     </row>
     <row r="59" spans="2:16" x14ac:dyDescent="0.2">
@@ -2974,7 +2974,7 @@
       </c>
       <c r="P59">
         <f ca="1"/>
-        <v>55</v>
+        <v>76</v>
       </c>
     </row>
     <row r="60" spans="2:16" x14ac:dyDescent="0.2">
@@ -3021,7 +3021,7 @@
       </c>
       <c r="P60">
         <f ca="1"/>
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="61" spans="2:16" x14ac:dyDescent="0.2">
@@ -3068,7 +3068,7 @@
       </c>
       <c r="P61">
         <f ca="1"/>
-        <v>73</v>
+        <v>35</v>
       </c>
     </row>
     <row r="62" spans="2:16" x14ac:dyDescent="0.2">
@@ -3115,7 +3115,7 @@
       </c>
       <c r="P62">
         <f ca="1"/>
-        <v>21</v>
+        <v>46</v>
       </c>
     </row>
     <row r="63" spans="2:16" x14ac:dyDescent="0.2">
@@ -3162,7 +3162,7 @@
       </c>
       <c r="P63">
         <f ca="1"/>
-        <v>71</v>
+        <v>42</v>
       </c>
     </row>
     <row r="64" spans="2:16" x14ac:dyDescent="0.2">
@@ -3209,7 +3209,7 @@
       </c>
       <c r="P64">
         <f ca="1"/>
-        <v>62</v>
+        <v>67</v>
       </c>
     </row>
     <row r="65" spans="2:16" x14ac:dyDescent="0.2">
@@ -3245,7 +3245,7 @@
       </c>
       <c r="L65">
         <f t="shared" ca="1" si="0"/>
-        <v>0.32790830944763094</v>
+        <v>0</v>
       </c>
       <c r="M65" t="s">
         <v>5</v>
@@ -3256,7 +3256,7 @@
       </c>
       <c r="P65">
         <f ca="1"/>
-        <v>12</v>
+        <v>28</v>
       </c>
     </row>
     <row r="66" spans="2:16" x14ac:dyDescent="0.2">
@@ -3292,7 +3292,7 @@
       </c>
       <c r="L66">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>5.9512135612594941E-3</v>
       </c>
       <c r="M66" t="s">
         <v>5</v>
@@ -3303,7 +3303,7 @@
       </c>
       <c r="P66">
         <f ca="1"/>
-        <v>25</v>
+        <v>4</v>
       </c>
     </row>
     <row r="67" spans="2:16" x14ac:dyDescent="0.2">
@@ -3350,7 +3350,7 @@
       </c>
       <c r="P67">
         <f ca="1"/>
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="68" spans="2:16" x14ac:dyDescent="0.2">
@@ -3386,7 +3386,7 @@
       </c>
       <c r="L68">
         <f t="shared" ca="1" si="0"/>
-        <v>0.38796979243088536</v>
+        <v>0</v>
       </c>
       <c r="M68" t="s">
         <v>5</v>
@@ -3397,7 +3397,7 @@
       </c>
       <c r="P68">
         <f ca="1"/>
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="69" spans="2:16" x14ac:dyDescent="0.2">
@@ -3444,7 +3444,7 @@
       </c>
       <c r="P69">
         <f ca="1"/>
-        <v>28</v>
+        <v>75</v>
       </c>
     </row>
     <row r="70" spans="2:16" x14ac:dyDescent="0.2">
@@ -3491,7 +3491,7 @@
       </c>
       <c r="P70">
         <f ca="1"/>
-        <v>45</v>
+        <v>58</v>
       </c>
     </row>
     <row r="71" spans="2:16" x14ac:dyDescent="0.2">
@@ -3527,7 +3527,7 @@
       </c>
       <c r="L71">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>0.42315170009057973</v>
       </c>
       <c r="M71" t="s">
         <v>5</v>
@@ -3538,7 +3538,7 @@
       </c>
       <c r="P71">
         <f ca="1"/>
-        <v>56</v>
+        <v>6</v>
       </c>
     </row>
     <row r="72" spans="2:16" x14ac:dyDescent="0.2">
@@ -3585,7 +3585,7 @@
       </c>
       <c r="P72">
         <f ca="1"/>
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="73" spans="2:16" x14ac:dyDescent="0.2">
@@ -3632,7 +3632,7 @@
       </c>
       <c r="P73">
         <f ca="1"/>
-        <v>54</v>
+        <v>30</v>
       </c>
     </row>
     <row r="74" spans="2:16" x14ac:dyDescent="0.2">
@@ -3679,7 +3679,7 @@
       </c>
       <c r="P74">
         <f ca="1"/>
-        <v>69</v>
+        <v>23</v>
       </c>
     </row>
     <row r="75" spans="2:16" x14ac:dyDescent="0.2">
@@ -3714,7 +3714,7 @@
         <v>1</v>
       </c>
       <c r="L75">
-        <f t="shared" ref="L75:L85" ca="1" si="2">IF(COUNTIF(O$10:O$29, P75)&gt;0, RAND()*0.5, 0)</f>
+        <f t="shared" ref="L75:L85" ca="1" si="2">IF(COUNTIF(O$10:O$19, P75)&gt;0, RAND()*0.5, 0)</f>
         <v>0</v>
       </c>
       <c r="M75" t="s">
@@ -3726,7 +3726,7 @@
       </c>
       <c r="P75">
         <f ca="1"/>
-        <v>37</v>
+        <v>68</v>
       </c>
     </row>
     <row r="76" spans="2:16" x14ac:dyDescent="0.2">
@@ -3773,7 +3773,7 @@
       </c>
       <c r="P76">
         <f ca="1"/>
-        <v>60</v>
+        <v>45</v>
       </c>
     </row>
     <row r="77" spans="2:16" x14ac:dyDescent="0.2">
@@ -3820,7 +3820,7 @@
       </c>
       <c r="P77">
         <f ca="1"/>
-        <v>67</v>
+        <v>43</v>
       </c>
     </row>
     <row r="78" spans="2:16" x14ac:dyDescent="0.2">
@@ -3867,7 +3867,7 @@
       </c>
       <c r="P78">
         <f ca="1"/>
-        <v>40</v>
+        <v>73</v>
       </c>
     </row>
     <row r="79" spans="2:16" x14ac:dyDescent="0.2">
@@ -3903,7 +3903,7 @@
       </c>
       <c r="L79">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>0.21558904229761766</v>
       </c>
       <c r="M79" t="s">
         <v>5</v>
@@ -3914,7 +3914,7 @@
       </c>
       <c r="P79">
         <f ca="1"/>
-        <v>29</v>
+        <v>1</v>
       </c>
     </row>
     <row r="80" spans="2:16" x14ac:dyDescent="0.2">
@@ -3961,7 +3961,7 @@
       </c>
       <c r="P80">
         <f ca="1"/>
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="81" spans="2:16" x14ac:dyDescent="0.2">
@@ -3997,7 +3997,7 @@
       </c>
       <c r="L81">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>0.12834380058220624</v>
       </c>
       <c r="M81" t="s">
         <v>5</v>
@@ -4008,7 +4008,7 @@
       </c>
       <c r="P81">
         <f ca="1"/>
-        <v>23</v>
+        <v>10</v>
       </c>
     </row>
     <row r="82" spans="2:16" x14ac:dyDescent="0.2">
@@ -4055,7 +4055,7 @@
       </c>
       <c r="P82">
         <f ca="1"/>
-        <v>49</v>
+        <v>56</v>
       </c>
     </row>
     <row r="83" spans="2:16" x14ac:dyDescent="0.2">
@@ -4091,7 +4091,7 @@
       </c>
       <c r="L83">
         <f t="shared" ca="1" si="2"/>
-        <v>0.41559988475236714</v>
+        <v>0</v>
       </c>
       <c r="M83" t="s">
         <v>5</v>
@@ -4102,7 +4102,7 @@
       </c>
       <c r="P83">
         <f ca="1"/>
-        <v>10</v>
+        <v>55</v>
       </c>
     </row>
     <row r="84" spans="2:16" x14ac:dyDescent="0.2">
@@ -4149,7 +4149,7 @@
       </c>
       <c r="P84">
         <f ca="1"/>
-        <v>22</v>
+        <v>61</v>
       </c>
     </row>
     <row r="85" spans="2:16" x14ac:dyDescent="0.2">
@@ -4185,7 +4185,7 @@
       </c>
       <c r="L85">
         <f t="shared" ca="1" si="2"/>
-        <v>0.11472345795510502</v>
+        <v>0</v>
       </c>
       <c r="M85" t="s">
         <v>5</v>
@@ -4196,11 +4196,10 @@
       </c>
       <c r="P85">
         <f ca="1"/>
-        <v>19</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>